<commit_message>
removed async and recursive code (eliminated cancel cunctionality) for better dev-ability. Also moved functions to main.py upload_files function
</commit_message>
<xml_diff>
--- a/logs/General Log/General-Log.xlsx
+++ b/logs/General Log/General-Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,6 +907,770 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:12:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ORM-0515839</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:12:51</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ORM-0515840</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:13:29</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ORM-0515839</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:13:31</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ORM-0515840</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:15:05</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ORM-0515839</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:15:07</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ORM-0515840</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:16:21</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ORM-0515848</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>201</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d5b10e4653161b72f1"},"data":{"type":"material","id":"asset:66f3c6d5b10e4653161b72f1","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d5b10e4653161b72f1"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c6d5b10e4653161b72f1","id":"asset:66f3c6d5b10e4653161b72f1","eid":"asset:66f3c6d5b10e4653161b72f1","name":"ORM-0515848","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:16:21.164Z","editedAt":"2024-09-25T08:16:21.164Z","type":"asset","digest":"38834240","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515848"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c6d5b10e4653161b72f2","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c6d5b10e4653161b72f2"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d5b10e4653161b72f1/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c6d5b10e4653161b72f1"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c6d5b10e4653161b72f2","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c6d5b10e4653161b72f2"},"attributes":{"type":"batch","eid":"batch:66f3c6d5b10e4653161b72f2","name":"ORM-0515848-001","digest":"48077144","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515848-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:16:21.480Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"78459056","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:66f3c6d5b10e4653161b72f1","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d5b10e4653161b72f1/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c6d5b10e4653161b72f1","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:16:24</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ORM-0515849</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>201</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d7a01482132101b337"},"data":{"type":"material","id":"asset:66f3c6d7a01482132101b337","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d7a01482132101b337"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c6d7a01482132101b337","id":"asset:66f3c6d7a01482132101b337","eid":"asset:66f3c6d7a01482132101b337","name":"ORM-0515849","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:16:23.917Z","editedAt":"2024-09-25T08:16:23.917Z","type":"asset","digest":"39131108","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515849"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c6d8a01482132101b338","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c6d8a01482132101b338"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d7a01482132101b337/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c6d7a01482132101b337"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c6d8a01482132101b338","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c6d8a01482132101b338"},"attributes":{"type":"batch","eid":"batch:66f3c6d8a01482132101b338","name":"ORM-0515849-001","digest":"86043289","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515849-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:16:24.220Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"78459056","fields":{}}},{"type":"materialDrawing","id":"asset:66f3c6d7a01482132101b337","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c6d7a01482132101b337/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c6d7a01482132101b337","type":"CHEMICAL_DRAWING"}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:22:12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ORM-0515850</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>201</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c833a01482132101b347"},"data":{"type":"material","id":"asset:66f3c833a01482132101b347","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c833a01482132101b347"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c833a01482132101b347","id":"asset:66f3c833a01482132101b347","eid":"asset:66f3c833a01482132101b347","name":"ORM-0515850","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:22:11.916Z","editedAt":"2024-09-25T08:22:11.916Z","type":"asset","digest":"51238311","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515850"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c834a01482132101b348","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c834a01482132101b348"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c833a01482132101b347/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c833a01482132101b347"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:66f3c833a01482132101b347","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c833a01482132101b347/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c833a01482132101b347","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:66f3c834a01482132101b348","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c834a01482132101b348"},"attributes":{"type":"batch","eid":"batch:66f3c834a01482132101b348","name":"ORM-0515850-001","digest":"16964069","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515850-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:22:12.229Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"61526003","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:22:15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ORM-0515851</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>201</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c837399ff04b78d3b950"},"data":{"type":"material","id":"asset:66f3c837399ff04b78d3b950","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c837399ff04b78d3b950"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c837399ff04b78d3b950","id":"asset:66f3c837399ff04b78d3b950","eid":"asset:66f3c837399ff04b78d3b950","name":"ORM-0515851","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:22:15.127Z","editedAt":"2024-09-25T08:22:15.127Z","type":"asset","digest":"76371280","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515851"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c837399ff04b78d3b951","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c837399ff04b78d3b951"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c837399ff04b78d3b950/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c837399ff04b78d3b950"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c837399ff04b78d3b951","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c837399ff04b78d3b951"},"attributes":{"type":"batch","eid":"batch:66f3c837399ff04b78d3b951","name":"ORM-0515851-001","digest":"65911264","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515851-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:22:15.310Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:66f3c837399ff04b78d3b950","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c837399ff04b78d3b950/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c837399ff04b78d3b950","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"61526003","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:25:15</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ORM-0515852</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>201</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8eaccf303112a9a6319"},"data":{"type":"material","id":"asset:66f3c8eaccf303112a9a6319","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8eaccf303112a9a6319"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c8eaccf303112a9a6319","id":"asset:66f3c8eaccf303112a9a6319","eid":"asset:66f3c8eaccf303112a9a6319","name":"ORM-0515852","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:25:14.449Z","editedAt":"2024-09-25T08:25:14.449Z","type":"asset","digest":"50162357","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515852"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c8eaccf303112a9a631a","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c8eaccf303112a9a631a"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8eaccf303112a9a6319/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c8eaccf303112a9a6319"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c8eaccf303112a9a631a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c8eaccf303112a9a631a"},"attributes":{"type":"batch","eid":"batch:66f3c8eaccf303112a9a631a","name":"ORM-0515852-001","digest":"94979605","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515852-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:25:14.924Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"48247138","fields":{}}},{"type":"materialDrawing","id":"asset:66f3c8eaccf303112a9a6319","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8eaccf303112a9a6319/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c8eaccf303112a9a6319","type":"CHEMICAL_DRAWING"}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:25:18</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ORM-0515853</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>201</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8ed8ac1f915a4ada772"},"data":{"type":"material","id":"asset:66f3c8ed8ac1f915a4ada772","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8ed8ac1f915a4ada772"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c8ed8ac1f915a4ada772","id":"asset:66f3c8ed8ac1f915a4ada772","eid":"asset:66f3c8ed8ac1f915a4ada772","name":"ORM-0515853","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:25:17.401Z","editedAt":"2024-09-25T08:25:17.401Z","type":"asset","digest":"27686644","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515853"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c8ed8ac1f915a4ada773","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c8ed8ac1f915a4ada773"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8ed8ac1f915a4ada772/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c8ed8ac1f915a4ada772"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c8ed8ac1f915a4ada773","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c8ed8ac1f915a4ada773"},"attributes":{"type":"batch","eid":"batch:66f3c8ed8ac1f915a4ada773","name":"ORM-0515853-001","digest":"90612978","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515853-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:25:17.893Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:66f3c8ed8ac1f915a4ada772","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c8ed8ac1f915a4ada772/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c8ed8ac1f915a4ada772","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"48247138","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:29:52</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ORM-0515854</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>201</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c9ff399ff04b78d3b952"},"data":{"type":"material","id":"asset:66f3c9ff399ff04b78d3b952","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c9ff399ff04b78d3b952"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3c9ff399ff04b78d3b952","id":"asset:66f3c9ff399ff04b78d3b952","eid":"asset:66f3c9ff399ff04b78d3b952","name":"ORM-0515854","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:29:51.259Z","editedAt":"2024-09-25T08:29:51.259Z","type":"asset","digest":"61891900","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515854"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3c9ff399ff04b78d3b953","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c9ff399ff04b78d3b953"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c9ff399ff04b78d3b952/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3c9ff399ff04b78d3b952"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3c9ff399ff04b78d3b953","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3c9ff399ff04b78d3b953"},"attributes":{"type":"batch","eid":"batch:66f3c9ff399ff04b78d3b953","name":"ORM-0515854-001","digest":"74433293","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515854-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:29:51.916Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"26314572","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:66f3c9ff399ff04b78d3b952","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3c9ff399ff04b78d3b952/drawing?format=cdxml"},"attributes":{"id":"asset:66f3c9ff399ff04b78d3b952","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:29:55</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ORM-0515855</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>201</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca02399ff04b78d3b954"},"data":{"type":"material","id":"asset:66f3ca02399ff04b78d3b954","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca02399ff04b78d3b954"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3ca02399ff04b78d3b954","id":"asset:66f3ca02399ff04b78d3b954","eid":"asset:66f3ca02399ff04b78d3b954","name":"ORM-0515855","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:29:54.458Z","editedAt":"2024-09-25T08:29:54.458Z","type":"asset","digest":"83080449","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515855"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3ca02399ff04b78d3b955","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca02399ff04b78d3b955"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca02399ff04b78d3b954/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3ca02399ff04b78d3b954"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:66f3ca02399ff04b78d3b954","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca02399ff04b78d3b954/drawing?format=cdxml"},"attributes":{"id":"asset:66f3ca02399ff04b78d3b954","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:66f3ca02399ff04b78d3b955","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca02399ff04b78d3b955"},"attributes":{"type":"batch","eid":"batch:66f3ca02399ff04b78d3b955","name":"ORM-0515855-001","digest":"99076106","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515855-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:29:54.923Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"26314572","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:31:32</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ORM-0515856</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>201</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca63399ff04b78d3b956"},"data":{"type":"material","id":"asset:66f3ca63399ff04b78d3b956","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca63399ff04b78d3b956"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3ca63399ff04b78d3b956","id":"asset:66f3ca63399ff04b78d3b956","eid":"asset:66f3ca63399ff04b78d3b956","name":"ORM-0515856","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:31:31.876Z","editedAt":"2024-09-25T08:31:31.876Z","type":"asset","digest":"31175883","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515856"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3ca64399ff04b78d3b957","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca64399ff04b78d3b957"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca63399ff04b78d3b956/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3ca63399ff04b78d3b956"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3ca64399ff04b78d3b957","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca64399ff04b78d3b957"},"attributes":{"type":"batch","eid":"batch:66f3ca64399ff04b78d3b957","name":"ORM-0515856-001","digest":"53712521","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515856-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:31:32.093Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:66f3ca63399ff04b78d3b956","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca63399ff04b78d3b956/drawing?format=cdxml"},"attributes":{"id":"asset:66f3ca63399ff04b78d3b956","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"27915298","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:31:35</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ORM-0515857</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>201</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca66b10e4653161b7309"},"data":{"type":"material","id":"asset:66f3ca66b10e4653161b7309","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca66b10e4653161b7309"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3ca66b10e4653161b7309","id":"asset:66f3ca66b10e4653161b7309","eid":"asset:66f3ca66b10e4653161b7309","name":"ORM-0515857","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:31:34.474Z","editedAt":"2024-09-25T08:31:34.474Z","type":"asset","digest":"40461342","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515857"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3ca66b10e4653161b730a","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca66b10e4653161b730a"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca66b10e4653161b7309/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3ca66b10e4653161b7309"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3ca66b10e4653161b730a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3ca66b10e4653161b730a"},"attributes":{"type":"batch","eid":"batch:66f3ca66b10e4653161b730a","name":"ORM-0515857-001","digest":"70452462","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515857-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:31:34.908Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:66f3ca66b10e4653161b7309","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3ca66b10e4653161b7309/drawing?format=cdxml"},"attributes":{"id":"asset:66f3ca66b10e4653161b7309","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"27915298","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:35:05</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ORM-0515858</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>201</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb38399ff04b78d3b95a"},"data":{"type":"material","id":"asset:66f3cb38399ff04b78d3b95a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb38399ff04b78d3b95a"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3cb38399ff04b78d3b95a","id":"asset:66f3cb38399ff04b78d3b95a","eid":"asset:66f3cb38399ff04b78d3b95a","name":"ORM-0515858","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:35:04.906Z","editedAt":"2024-09-25T08:35:04.906Z","type":"asset","digest":"76671961","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515858"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3cb39399ff04b78d3b95b","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cb39399ff04b78d3b95b"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb38399ff04b78d3b95a/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3cb38399ff04b78d3b95a"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3cb39399ff04b78d3b95b","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cb39399ff04b78d3b95b"},"attributes":{"type":"batch","eid":"batch:66f3cb39399ff04b78d3b95b","name":"ORM-0515858-001","digest":"25909751","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515858-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:35:05.166Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"25407789","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:66f3cb38399ff04b78d3b95a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb38399ff04b78d3b95a/drawing?format=cdxml"},"attributes":{"id":"asset:66f3cb38399ff04b78d3b95a","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:35:08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ORM-0515859</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>201</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb3b399ff04b78d3b95c"},"data":{"type":"material","id":"asset:66f3cb3b399ff04b78d3b95c","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb3b399ff04b78d3b95c"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3cb3b399ff04b78d3b95c","id":"asset:66f3cb3b399ff04b78d3b95c","eid":"asset:66f3cb3b399ff04b78d3b95c","name":"ORM-0515859","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:35:07.478Z","editedAt":"2024-09-25T08:35:07.478Z","type":"asset","digest":"12743630","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515859"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3cb3b399ff04b78d3b95d","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cb3b399ff04b78d3b95d"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb3b399ff04b78d3b95c/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3cb3b399ff04b78d3b95c"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:66f3cb3b399ff04b78d3b95c","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cb3b399ff04b78d3b95c/drawing?format=cdxml"},"attributes":{"id":"asset:66f3cb3b399ff04b78d3b95c","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:66f3cb3b399ff04b78d3b95d","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cb3b399ff04b78d3b95d"},"attributes":{"type":"batch","eid":"batch:66f3cb3b399ff04b78d3b95d","name":"ORM-0515859-001","digest":"43866544","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515859-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:35:07.911Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"25407789","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:37:29</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ORM-0515860</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>201</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbc8b10e4653161b730b"},"data":{"type":"material","id":"asset:66f3cbc8b10e4653161b730b","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbc8b10e4653161b730b"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3cbc8b10e4653161b730b","id":"asset:66f3cbc8b10e4653161b730b","eid":"asset:66f3cbc8b10e4653161b730b","name":"ORM-0515860","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-09-25T08:37:28.263Z","editedAt":"2024-09-25T08:37:28.263Z","type":"asset","digest":"74629343","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515860"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3cbc8b10e4653161b730c","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cbc8b10e4653161b730c"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbc8b10e4653161b730b/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3cbc8b10e4653161b730b"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:66f3cbc8b10e4653161b730b","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbc8b10e4653161b730b/drawing?format=cdxml"},"attributes":{"id":"asset:66f3cbc8b10e4653161b730b","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:66f3cbc8b10e4653161b730c","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cbc8b10e4653161b730c"},"attributes":{"type":"batch","eid":"batch:66f3cbc8b10e4653161b730c","name":"ORM-0515860-001","digest":"24931436","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0515860-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:37:28.909Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"97254194","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-09-25 11:37:32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ORM-0515861</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>201</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbcbccf303112a9a6325"},"data":{"type":"material","id":"asset:66f3cbcbccf303112a9a6325","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbcbccf303112a9a6325"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"66f3cbcbccf303112a9a6325","id":"asset:66f3cbcbccf303112a9a6325","eid":"asset:66f3cbcbccf303112a9a6325","name":"ORM-0515861","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-09-25T08:37:31.457Z","editedAt":"2024-09-25T08:37:31.457Z","type":"asset","digest":"51579799","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0515861"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:66f3cbcbccf303112a9a6326","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cbcbccf303112a9a6326"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbcbccf303112a9a6325/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:66f3cbcbccf303112a9a6325"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:66f3cbcbccf303112a9a6326","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:66f3cbcbccf303112a9a6326"},"attributes":{"type":"batch","eid":"batch:66f3cbcbccf303112a9a6326","name":"ORM-0515861-001","digest":"54944541","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0515861-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-09-25T08:37:31.903Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:66f3cbcbccf303112a9a6325","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:66f3cbcbccf303112a9a6325/drawing?format=cdxml"},"attributes":{"id":"asset:66f3cbcbccf303112a9a6325","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"97254194","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fetches materials table and user can select project
</commit_message>
<xml_diff>
--- a/logs/General Log/General-Log.xlsx
+++ b/logs/General Log/General-Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,6 +2047,86 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:12:33</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ORM-0516002</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>201</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f47701a12207a92bcb000"},"data":{"type":"material","id":"asset:671f47701a12207a92bcb000","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f47701a12207a92bcb000"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f47701a12207a92bcb000","id":"asset:671f47701a12207a92bcb000","eid":"asset:671f47701a12207a92bcb000","name":"ORM-0516002","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T08:12:33.005Z","editedAt":"2024-10-28T08:12:33.005Z","type":"asset","digest":"16083839","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516002"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f47711a12207a92bcb001","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f47711a12207a92bcb001"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f47701a12207a92bcb000/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f47701a12207a92bcb000"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f47711a12207a92bcb001","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f47711a12207a92bcb001"},"attributes":{"type":"batch","eid":"batch:671f47711a12207a92bcb001","name":"ORM-0516002-001","digest":"73997506","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516002-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:12:33.547Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f47701a12207a92bcb000","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f47701a12207a92bcb000/drawing?format=cdxml"},"attributes":{"id":"asset:671f47701a12207a92bcb000","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"13184553","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:12:37</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ORM-0516003</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>201</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4774bc105f6067d3957e"},"data":{"type":"material","id":"asset:671f4774bc105f6067d3957e","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4774bc105f6067d3957e"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4774bc105f6067d3957e","id":"asset:671f4774bc105f6067d3957e","eid":"asset:671f4774bc105f6067d3957e","name":"ORM-0516003","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T08:12:36.905Z","editedAt":"2024-10-28T08:12:36.905Z","type":"asset","digest":"38794071","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516003"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4775bc105f6067d3957f","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4775bc105f6067d3957f"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4774bc105f6067d3957e/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4774bc105f6067d3957e"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f4775bc105f6067d3957f","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4775bc105f6067d3957f"},"attributes":{"type":"batch","eid":"batch:671f4775bc105f6067d3957f","name":"ORM-0516003-001","digest":"32351343","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0516003-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:12:37.534Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"13184553","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:671f4774bc105f6067d3957e","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4774bc105f6067d3957e/drawing?format=cdxml"},"attributes":{"id":"asset:671f4774bc105f6067d3957e","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
library ID input and mapping to payload
</commit_message>
<xml_diff>
--- a/logs/General Log/General-Log.xlsx
+++ b/logs/General Log/General-Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2127,6 +2127,406 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:17:42</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ORM-0516004</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>201</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a4b0480736afa1ed2d"},"data":{"type":"material","id":"asset:671f48a4b0480736afa1ed2d","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a4b0480736afa1ed2d"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f48a4b0480736afa1ed2d","id":"asset:671f48a4b0480736afa1ed2d","eid":"asset:671f48a4b0480736afa1ed2d","name":"ORM-0516004","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T08:17:41.024Z","editedAt":"2024-10-28T08:17:41.024Z","type":"asset","digest":"33984483","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516004"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f48a5b0480736afa1ed2e","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f48a5b0480736afa1ed2e"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a4b0480736afa1ed2d/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f48a4b0480736afa1ed2d"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f48a5b0480736afa1ed2e","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f48a5b0480736afa1ed2e"},"attributes":{"type":"batch","eid":"batch:671f48a5b0480736afa1ed2e","name":"ORM-0516004-001","digest":"38748822","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516004-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:17:41.551Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f48a4b0480736afa1ed2d","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a4b0480736afa1ed2d/drawing?format=cdxml"},"attributes":{"id":"asset:671f48a4b0480736afa1ed2d","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"11206735","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:17:45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ORM-0516005</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>201</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a8b0480736afa1ed2f"},"data":{"type":"material","id":"asset:671f48a8b0480736afa1ed2f","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a8b0480736afa1ed2f"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f48a8b0480736afa1ed2f","id":"asset:671f48a8b0480736afa1ed2f","eid":"asset:671f48a8b0480736afa1ed2f","name":"ORM-0516005","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T08:17:44.527Z","editedAt":"2024-10-28T08:17:44.527Z","type":"asset","digest":"54014979","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516005"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f48a8b0480736afa1ed30","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f48a8b0480736afa1ed30"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a8b0480736afa1ed2f/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f48a8b0480736afa1ed2f"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f48a8b0480736afa1ed30","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f48a8b0480736afa1ed30"},"attributes":{"type":"batch","eid":"batch:671f48a8b0480736afa1ed30","name":"ORM-0516005-001","digest":"57597351","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0516005-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:17:44.864Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"11206735","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:671f48a8b0480736afa1ed2f","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f48a8b0480736afa1ed2f/drawing?format=cdxml"},"attributes":{"id":"asset:671f48a8b0480736afa1ed2f","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:22:18</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ORM-0516006</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>201</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49b91a12207a92bcb002"},"data":{"type":"material","id":"asset:671f49b91a12207a92bcb002","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49b91a12207a92bcb002"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f49b91a12207a92bcb002","id":"asset:671f49b91a12207a92bcb002","eid":"asset:671f49b91a12207a92bcb002","name":"ORM-0516006","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T08:22:18.045Z","editedAt":"2024-10-28T08:22:18.045Z","type":"asset","digest":"81887489","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516006"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f49ba1a12207a92bcb003","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f49ba1a12207a92bcb003"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49b91a12207a92bcb002/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f49b91a12207a92bcb002"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f49ba1a12207a92bcb003","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f49ba1a12207a92bcb003"},"attributes":{"type":"batch","eid":"batch:671f49ba1a12207a92bcb003","name":"ORM-0516006-001","digest":"67763751","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516006-001"},"Project":{"value":"TRPA1"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:22:18.540Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f49b91a12207a92bcb002","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49b91a12207a92bcb002/drawing?format=cdxml"},"attributes":{"id":"asset:671f49b91a12207a92bcb002","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"64278126","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:22:23</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ORM-0516007</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>201</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49bdb0480736afa1ed31"},"data":{"type":"material","id":"asset:671f49bdb0480736afa1ed31","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49bdb0480736afa1ed31"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f49bdb0480736afa1ed31","id":"asset:671f49bdb0480736afa1ed31","eid":"asset:671f49bdb0480736afa1ed31","name":"ORM-0516007","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T08:22:22.001Z","editedAt":"2024-10-28T08:22:22.001Z","type":"asset","digest":"67739634","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516007"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f49beb0480736afa1ed32","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f49beb0480736afa1ed32"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49bdb0480736afa1ed31/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f49bdb0480736afa1ed31"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f49beb0480736afa1ed32","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f49beb0480736afa1ed32"},"attributes":{"type":"batch","eid":"batch:671f49beb0480736afa1ed32","name":"ORM-0516007-001","digest":"39670267","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Name":{"value":"ORM-0516007-001"},"Project":{"value":"TRPA1"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:22:22.538Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f49bdb0480736afa1ed31","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f49bdb0480736afa1ed31/drawing?format=cdxml"},"attributes":{"id":"asset:671f49bdb0480736afa1ed31","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"64278126","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:30:47</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ORM-0516008</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>201</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bb6aee6dd75754a8e07"},"data":{"type":"material","id":"asset:671f4bb6aee6dd75754a8e07","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bb6aee6dd75754a8e07"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4bb6aee6dd75754a8e07","id":"asset:671f4bb6aee6dd75754a8e07","eid":"asset:671f4bb6aee6dd75754a8e07","name":"ORM-0516008","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T08:30:47.073Z","editedAt":"2024-10-28T08:30:47.073Z","type":"asset","digest":"75331620","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516008"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4bb7aee6dd75754a8e08","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4bb7aee6dd75754a8e08"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bb6aee6dd75754a8e07/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4bb6aee6dd75754a8e07"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f4bb7aee6dd75754a8e08","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4bb7aee6dd75754a8e08"},"attributes":{"type":"batch","eid":"batch:671f4bb7aee6dd75754a8e08","name":"ORM-0516008-001","digest":"94120596","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Library ID":{"value":"test"},"Name":{"value":"ORM-0516008-001"},"Project":{"value":"TRPA1"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:30:47.514Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"38038242","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:671f4bb6aee6dd75754a8e07","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bb6aee6dd75754a8e07/drawing?format=cdxml"},"attributes":{"id":"asset:671f4bb6aee6dd75754a8e07","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:30:51</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ORM-0516009</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>201</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bbab0480736afa1ed33"},"data":{"type":"material","id":"asset:671f4bbab0480736afa1ed33","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bbab0480736afa1ed33"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4bbab0480736afa1ed33","id":"asset:671f4bbab0480736afa1ed33","eid":"asset:671f4bbab0480736afa1ed33","name":"ORM-0516009","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T08:30:50.423Z","editedAt":"2024-10-28T08:30:50.423Z","type":"asset","digest":"82903810","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516009"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4bbab0480736afa1ed34","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4bbab0480736afa1ed34"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bbab0480736afa1ed33/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4bbab0480736afa1ed33"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:671f4bbab0480736afa1ed33","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4bbab0480736afa1ed33/drawing?format=cdxml"},"attributes":{"id":"asset:671f4bbab0480736afa1ed33","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"38038242","fields":{}}},{"type":"material","id":"batch:671f4bbab0480736afa1ed34","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4bbab0480736afa1ed34"},"attributes":{"type":"batch","eid":"batch:671f4bbab0480736afa1ed34","name":"ORM-0516009-001","digest":"51972337","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Library ID":{"value":"test"},"Name":{"value":"ORM-0516009-001"},"Project":{"value":"TRPA1"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:30:50.677Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:39:18</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ORM-0516010</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>201</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db5aee6dd75754a8e09"},"data":{"type":"material","id":"asset:671f4db5aee6dd75754a8e09","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db5aee6dd75754a8e09"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4db5aee6dd75754a8e09","id":"asset:671f4db5aee6dd75754a8e09","eid":"asset:671f4db5aee6dd75754a8e09","name":"ORM-0516010","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T08:39:17.468Z","editedAt":"2024-10-28T08:39:17.468Z","type":"asset","digest":"63825572","fields":{"Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516010"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4db5aee6dd75754a8e0a","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4db5aee6dd75754a8e0a"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db5aee6dd75754a8e09/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4db5aee6dd75754a8e09"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f4db5aee6dd75754a8e0a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4db5aee6dd75754a8e0a"},"attributes":{"type":"batch","eid":"batch:671f4db5aee6dd75754a8e0a","name":"ORM-0516010-001","digest":"81398182","fields":{"Batch Chemical Name":{"value":"2-[({4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl}methyl)(methyl)amino]-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516010-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:39:17.773Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f4db5aee6dd75754a8e09","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db5aee6dd75754a8e09/drawing?format=cdxml"},"attributes":{"id":"asset:671f4db5aee6dd75754a8e09","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"61458965","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:39:21</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ORM-0516011</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>201</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db8b1b4403b714883a6"},"data":{"type":"material","id":"asset:671f4db8b1b4403b714883a6","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db8b1b4403b714883a6"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4db8b1b4403b714883a6","id":"asset:671f4db8b1b4403b714883a6","eid":"asset:671f4db8b1b4403b714883a6","name":"ORM-0516011","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T08:39:21.016Z","editedAt":"2024-10-28T08:39:21.016Z","type":"asset","digest":"49838842","fields":{"Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516011"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4db9b1b4403b714883a7","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4db9b1b4403b714883a7"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db8b1b4403b714883a6/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4db8b1b4403b714883a6"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f4db9b1b4403b714883a7","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4db9b1b4403b714883a7"},"attributes":{"type":"batch","eid":"batch:671f4db9b1b4403b714883a7","name":"ORM-0516011-001","digest":"75355789","fields":{"Batch Chemical Name":{"value":"2-[1-(aminomethyl)cyclopropyl]-1-{2-[1-(2-methoxyethyl)-1H-imidazol-2-yl]-3,3-dimethylazetidin-1-yl}ethan-1-one hydrobromide, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516011-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:39:21.529Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f4db8b1b4403b714883a6","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4db8b1b4403b714883a6/drawing?format=cdxml"},"attributes":{"id":"asset:671f4db8b1b4403b714883a6","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"61458965","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:43:15</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ORM-0516012</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MCULE-2227031507</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>C21H17CLN2O2</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>201</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea26395b975bca22f6e"},"data":{"type":"material","id":"asset:671f4ea26395b975bca22f6e","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea26395b975bca22f6e"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4ea26395b975bca22f6e","id":"asset:671f4ea26395b975bca22f6e","eid":"asset:671f4ea26395b975bca22f6e","name":"ORM-0516012","synonyms":["C(=O)(NNC(=O)CC1CCC(C2CCCCC2)CC1)C1CCC(CC1)CL","C21H17CLN2O2"],"description":"","createdAt":"2024-10-28T08:43:14.577Z","editedAt":"2024-10-28T08:43:14.577Z","type":"asset","digest":"51718638","fields":{"Chemical Name":{"value":"2-{[1,1'-biphenyl]-4-yl}-N'-(4-chlorobenzoyl)acetohydrazide"},"Description":{"value":""},"Exact Mass":{"value":"364.09786"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;21&lt;/sub&gt;H&lt;sub&gt;17&lt;/sub&gt;ClN&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"364.83 g/mol"},"Name":{"value":"ORM-0516012"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4ea26395b975bca22f6f","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4ea26395b975bca22f6f"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea26395b975bca22f6e/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4ea26395b975bca22f6e"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:671f4ea26395b975bca22f6e","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea26395b975bca22f6e/drawing?format=cdxml"},"attributes":{"id":"asset:671f4ea26395b975bca22f6e","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:671f4ea26395b975bca22f6f","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4ea26395b975bca22f6f"},"attributes":{"type":"batch","eid":"batch:671f4ea26395b975bca22f6f","name":"ORM-0516012-001","digest":"28042261","fields":{"Batch Chemical Name":{"value":"2-{[1,1'-biphenyl]-4-yl}-N'-(4-chlorobenzoyl)acetohydrazide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;21&lt;/sub&gt;H&lt;sub&gt;17&lt;/sub&gt;ClN&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"364.83 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516012-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:43:14.874Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"81258343","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-10-28 10:43:18</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ORM-0516013</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MCULE-3988458386</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>C16H14CLN5O</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>201</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea61a12207a92bcb004"},"data":{"type":"material","id":"asset:671f4ea61a12207a92bcb004","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea61a12207a92bcb004"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f4ea61a12207a92bcb004","id":"asset:671f4ea61a12207a92bcb004","eid":"asset:671f4ea61a12207a92bcb004","name":"ORM-0516013","synonyms":["C1(C([NH]NN1)NC1CCC(CL)CC1)C(=O)NC1CCC(CC1)C","C16H14CLN5O"],"description":"","createdAt":"2024-10-28T08:43:18.149Z","editedAt":"2024-10-28T08:43:18.149Z","type":"asset","digest":"34482990","fields":{"Chemical Name":{"value":"5-[(4-chlorophenyl)amino]-N-(4-methylphenyl)-1H-1,2,3-triazole-4-carboxamide"},"Description":{"value":""},"Exact Mass":{"value":"327.08869"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;16&lt;/sub&gt;H&lt;sub&gt;14&lt;/sub&gt;ClN&lt;sub&gt;5&lt;/sub&gt;O"},"Molecular Weight":{"value":"327.77 g/mol"},"Name":{"value":"ORM-0516013"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f4ea61a12207a92bcb005","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4ea61a12207a92bcb005"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea61a12207a92bcb004/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f4ea61a12207a92bcb004"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:671f4ea61a12207a92bcb004","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f4ea61a12207a92bcb004/drawing?format=cdxml"},"attributes":{"id":"asset:671f4ea61a12207a92bcb004","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:671f4ea61a12207a92bcb005","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f4ea61a12207a92bcb005"},"attributes":{"type":"batch","eid":"batch:671f4ea61a12207a92bcb005","name":"ORM-0516013-001","digest":"93426211","fields":{"Batch Chemical Name":{"value":"5-[(4-chlorophenyl)amino]-N-(4-methylphenyl)-1H-1,2,3-triazole-4-carboxamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;16&lt;/sub&gt;H&lt;sub&gt;14&lt;/sub&gt;ClN&lt;sub&gt;5&lt;/sub&gt;O"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"327.77 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516013-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T08:43:18.520Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"81258343","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
removed chemical name, assigned by elwis automatically
</commit_message>
<xml_diff>
--- a/logs/General Log/General-Log.xlsx
+++ b/logs/General Log/General-Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2527,6 +2527,206 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-10-28 11:06:19</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ORM-0516014</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>MolPort-009-747-996</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>C14H11N3O2S</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MOLPORT/molport_test.sdf</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>201</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f540abc105f6067d39580"},"data":{"type":"material","id":"asset:671f540abc105f6067d39580","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f540abc105f6067d39580"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f540abc105f6067d39580","id":"asset:671f540abc105f6067d39580","eid":"asset:671f540abc105f6067d39580","name":"ORM-0516014","synonyms":["N1C(ONC1C)C1CCC(NC(=O)C2SCCC2)CC1","C14H11N3O2S"],"description":"","createdAt":"2024-10-28T09:06:18.567Z","editedAt":"2024-10-28T09:06:18.567Z","type":"asset","digest":"31900071","fields":{"Chemical Name":{"value":"N-[4-(3-methyl-1,2,4-oxadiazol-5-yl)phenyl]thiophene-2-carboxamide"},"Description":{"value":""},"Exact Mass":{"value":"285.0572"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;14&lt;/sub&gt;H&lt;sub&gt;11&lt;/sub&gt;N&lt;sub&gt;3&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;S"},"Molecular Weight":{"value":"285.32 g/mol"},"Name":{"value":"ORM-0516014"},"Stereochemistry":{"value":"achiral"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f540abc105f6067d39581","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f540abc105f6067d39581"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f540abc105f6067d39580/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f540abc105f6067d39580"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f540abc105f6067d39581","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f540abc105f6067d39581"},"attributes":{"type":"batch","eid":"batch:671f540abc105f6067d39581","name":"ORM-0516014-001","digest":"16551587","fields":{"Batch Chemical Name":{"value":"N-[4-(3-methyl-1,2,4-oxadiazol-5-yl)phenyl]thiophene-2-carboxamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;14&lt;/sub&gt;H&lt;sub&gt;11&lt;/sub&gt;N&lt;sub&gt;3&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;S"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"285.32 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516014-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T09:06:18.891Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f540abc105f6067d39580","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f540abc105f6067d39580/drawing?format=cdxml"},"attributes":{"id":"asset:671f540abc105f6067d39580","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"15127052","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-10-28 11:09:41</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ORM-0516015</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>201</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d46395b975bca22f75"},"data":{"type":"material","id":"asset:671f54d46395b975bca22f75","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d46395b975bca22f75"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f54d46395b975bca22f75","id":"asset:671f54d46395b975bca22f75","eid":"asset:671f54d46395b975bca22f75","name":"ORM-0516015","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T09:09:40.547Z","editedAt":"2024-10-28T09:09:40.547Z","type":"asset","digest":"54222663","fields":{"Chemical Name":{"value":"2-(((4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl)methyl)(methyl)amino)-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516015"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f54d46395b975bca22f76","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f54d46395b975bca22f76"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d46395b975bca22f75/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f54d46395b975bca22f75"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:671f54d46395b975bca22f75","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d46395b975bca22f75/drawing?format=cdxml"},"attributes":{"id":"asset:671f54d46395b975bca22f75","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"87955301","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"material","id":"batch:671f54d46395b975bca22f76","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f54d46395b975bca22f76"},"attributes":{"type":"batch","eid":"batch:671f54d46395b975bca22f76","name":"ORM-0516015-001","digest":"75127726","fields":{"Batch Chemical Name":{"value":"2-(((4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl)methyl)(methyl)amino)-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516015-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T09:09:40.795Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-10-28 11:09:44</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ORM-0516016</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>201</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d7bc105f6067d39582"},"data":{"type":"material","id":"asset:671f54d7bc105f6067d39582","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d7bc105f6067d39582"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f54d7bc105f6067d39582","id":"asset:671f54d7bc105f6067d39582","eid":"asset:671f54d7bc105f6067d39582","name":"ORM-0516016","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T09:09:43.906Z","editedAt":"2024-10-28T09:09:43.906Z","type":"asset","digest":"33035143","fields":{"Chemical Name":{"value":"2-(1-(aminomethyl)cyclopropyl)-1-(2-(1-(2-methoxyethyl)-1H-imidazol-2-yl)-3,3-dimethylazetidin-1-yl)ethan-1-one"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516016"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f54d8bc105f6067d39583","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f54d8bc105f6067d39583"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d7bc105f6067d39582/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f54d7bc105f6067d39582"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f54d8bc105f6067d39583","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f54d8bc105f6067d39583"},"attributes":{"type":"batch","eid":"batch:671f54d8bc105f6067d39583","name":"ORM-0516016-001","digest":"13092146","fields":{"Batch Chemical Name":{"value":"2-(1-(aminomethyl)cyclopropyl)-1-(2-(1-(2-methoxyethyl)-1H-imidazol-2-yl)-3,3-dimethylazetidin-1-yl)ethan-1-one, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516016-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T09:09:44.125Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f54d7bc105f6067d39582","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f54d7bc105f6067d39582/drawing?format=cdxml"},"attributes":{"id":"asset:671f54d7bc105f6067d39582","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"87955301","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-10-28 11:11:08</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ORM-0516017</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>201</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552b6395b975bca22f77"},"data":{"type":"material","id":"asset:671f552b6395b975bca22f77","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552b6395b975bca22f77"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f552b6395b975bca22f77","id":"asset:671f552b6395b975bca22f77","eid":"asset:671f552b6395b975bca22f77","name":"ORM-0516017","synonyms":["CN(CC(=O)NC1C(CL)CCCC1CL)CC1NC(N)C2C(C)C(C)SC2N1","C18H19CL2N5OS"],"description":"","createdAt":"2024-10-28T09:11:07.783Z","editedAt":"2024-10-28T09:11:07.783Z","type":"asset","digest":"88092569","fields":{"Chemical Name":{"value":"2-(((4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl)methyl)(methyl)amino)-N-(2,6-dichlorophenyl)acetamide"},"Description":{"value":""},"Exact Mass":{"value":"423.06874"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Molecular Weight":{"value":"424.34 g/mol"},"Name":{"value":"ORM-0516017"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f552b6395b975bca22f78","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f552b6395b975bca22f78"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552b6395b975bca22f77/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f552b6395b975bca22f77"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"materialDrawing","id":"asset:671f552b6395b975bca22f77","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552b6395b975bca22f77/drawing?format=cdxml"},"attributes":{"id":"asset:671f552b6395b975bca22f77","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"batch:671f552b6395b975bca22f78","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f552b6395b975bca22f78"},"attributes":{"type":"batch","eid":"batch:671f552b6395b975bca22f78","name":"ORM-0516017-001","digest":"64567284","fields":{"Batch Chemical Name":{"value":"2-(((4-amino-5,6-dimethylthieno[2,3-d]pyrimidin-2-yl)methyl)(methyl)amino)-N-(2,6-dichlorophenyl)acetamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;18&lt;/sub&gt;H&lt;sub&gt;19&lt;/sub&gt;Cl&lt;sub&gt;2&lt;/sub&gt;N&lt;sub&gt;5&lt;/sub&gt;OS"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"424.34 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516017-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T09:11:08.029Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"68126978","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-10-28 11:11:11</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ORM-0516018</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>201</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552e1a12207a92bcb007"},"data":{"type":"material","id":"asset:671f552e1a12207a92bcb007","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552e1a12207a92bcb007"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671f552e1a12207a92bcb007","id":"asset:671f552e1a12207a92bcb007","eid":"asset:671f552e1a12207a92bcb007","name":"ORM-0516018","synonyms":["COCCN1CCNC1C1N(CC1(C)C)C(=O)CC1(CN)CC1","C17H28N4O2"],"description":"","createdAt":"2024-10-28T09:11:10.782Z","editedAt":"2024-10-28T09:11:10.782Z","type":"asset","digest":"41788883","fields":{"Chemical Name":{"value":"2-(1-(aminomethyl)cyclopropyl)-1-(2-(1-(2-methoxyethyl)-1H-imidazol-2-yl)-3,3-dimethylazetidin-1-yl)ethan-1-one"},"Description":{"value":""},"Exact Mass":{"value":"320.22123"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"320.44 g/mol"},"Name":{"value":"ORM-0516018"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671f552e1a12207a92bcb008","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f552e1a12207a92bcb008"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552e1a12207a92bcb007/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671f552e1a12207a92bcb007"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671f552e1a12207a92bcb008","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671f552e1a12207a92bcb008"},"attributes":{"type":"batch","eid":"batch:671f552e1a12207a92bcb008","name":"ORM-0516018-001","digest":"58492800","fields":{"Batch Chemical Name":{"value":"2-(1-(aminomethyl)cyclopropyl)-1-(2-(1-(2-methoxyethyl)-1H-imidazol-2-yl)-3,3-dimethylazetidin-1-yl)ethan-1-one, hydrogen bromide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;17&lt;/sub&gt;H&lt;sub&gt;28&lt;/sub&gt;N&lt;sub&gt;4&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;&amp;middot;BRH"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"359.901 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516018-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T09:11:11.028Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"materialDrawing","id":"asset:671f552e1a12207a92bcb007","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671f552e1a12207a92bcb007/drawing?format=cdxml"},"attributes":{"id":"asset:671f552e1a12207a92bcb007","type":"CHEMICAL_DRAWING"}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"68126978","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated todo in readme
</commit_message>
<xml_diff>
--- a/logs/General Log/General-Log.xlsx
+++ b/logs/General Log/General-Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4845,6 +4845,86 @@
         </is>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-10-28 19:27:52</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>ORM-0516056</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>MCULE-2227031507</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>C21H17CLN2O2</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>201</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc997b0480736afa1ed64"},"data":{"type":"material","id":"asset:671fc997b0480736afa1ed64","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc997b0480736afa1ed64"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671fc997b0480736afa1ed64","id":"asset:671fc997b0480736afa1ed64","eid":"asset:671fc997b0480736afa1ed64","name":"ORM-0516056","synonyms":["C(=O)(NNC(=O)CC1CCC(C2CCCCC2)CC1)C1CCC(CC1)CL","C21H17CLN2O2"],"description":"","createdAt":"2024-10-28T17:27:51.830Z","editedAt":"2024-10-28T17:27:51.830Z","type":"asset","digest":"66868543","fields":{"Chemical Name":{"value":"N'-(2-([1,1'-biphenyl]-4-yl)acetyl)-4-chlorobenzohydrazide"},"Description":{"value":""},"Exact Mass":{"value":"364.09786"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;21&lt;/sub&gt;H&lt;sub&gt;17&lt;/sub&gt;ClN&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Molecular Weight":{"value":"364.83 g/mol"},"Name":{"value":"ORM-0516056"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671fc998b0480736afa1ed65","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671fc998b0480736afa1ed65"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc997b0480736afa1ed64/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671fc997b0480736afa1ed64"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671fc998b0480736afa1ed65","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671fc998b0480736afa1ed65"},"attributes":{"type":"batch","eid":"batch:671fc998b0480736afa1ed65","name":"ORM-0516056-001","digest":"83571980","fields":{"Batch Chemical Name":{"value":"N'-(2-([1,1'-biphenyl]-4-yl)acetyl)-4-chlorobenzohydrazide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;21&lt;/sub&gt;H&lt;sub&gt;17&lt;/sub&gt;ClN&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;2&lt;/sub&gt;"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"364.83 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516056-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T17:27:52.147Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Supplier Name":{"value":"Chembridge"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"59951413","fields":{}}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}},{"type":"materialDrawing","id":"asset:671fc997b0480736afa1ed64","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc997b0480736afa1ed64/drawing?format=cdxml"},"attributes":{"id":"asset:671fc997b0480736afa1ed64","type":"CHEMICAL_DRAWING"}}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-10-28 19:27:56</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ORM-0516057</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>MCULE-3988458386</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>C16H14CLN5O</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>201</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc99b1a12207a92bcb05a"},"data":{"type":"material","id":"asset:671fc99b1a12207a92bcb05a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc99b1a12207a92bcb05a"},"attributes":{"library":"Compounds","assetTypeId":"5d6e0287ee35880008c18db5","assetId":"671fc99b1a12207a92bcb05a","id":"asset:671fc99b1a12207a92bcb05a","eid":"asset:671fc99b1a12207a92bcb05a","name":"ORM-0516057","synonyms":["C1(C([NH]NN1)NC1CCC(CL)CC1)C(=O)NC1CCC(CC1)C","C16H14CLN5O"],"description":"","createdAt":"2024-10-28T17:27:55.840Z","editedAt":"2024-10-28T17:27:55.840Z","type":"asset","digest":"93385593","fields":{"Chemical Name":{"value":"5-((4-chlorophenyl)amino)-N-(p-tolyl)-1H-1,2,3-triazole-4-carboxamide"},"Description":{"value":""},"Exact Mass":{"value":"327.08869"},"Material Library Type":{"value":"Compounds"},"Molecular Formula":{"value":"C&lt;sub&gt;16&lt;/sub&gt;H&lt;sub&gt;14&lt;/sub&gt;ClN&lt;sub&gt;5&lt;/sub&gt;O"},"Molecular Weight":{"value":"327.77 g/mol"},"Name":{"value":"ORM-0516057"},"Stereochemistry":{"value":"No stereochemistry"}},"flags":{"canTrash":true}},"relationships":{"batches":{"data":[{"type":"material","id":"batch:671fc99c1a12207a92bcb05b","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671fc99c1a12207a92bcb05b"}}}]},"ancestors":{"data":[{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","meta":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"}}}]},"chemicalDrawing":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc99b1a12207a92bcb05a/drawing?format=cdxml"},"data":{"type":"materialDrawing","id":"asset:671fc99b1a12207a92bcb05a"}},"createdBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"editedBy":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}},"owner":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"data":{"type":"user","id":"114"}}}},"included":[{"type":"material","id":"batch:671fc99c1a12207a92bcb05b","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/batch:671fc99c1a12207a92bcb05b"},"attributes":{"type":"batch","eid":"batch:671fc99c1a12207a92bcb05b","name":"ORM-0516057-001","digest":"59455064","fields":{"Batch Chemical Name":{"value":"5-((4-chlorophenyl)amino)-N-(p-tolyl)-1H-1,2,3-triazole-4-carboxamide"},"Batch Molecular Formula":{"value":"C&lt;sub&gt;16&lt;/sub&gt;H&lt;sub&gt;14&lt;/sub&gt;ClN&lt;sub&gt;5&lt;/sub&gt;O"},"Batch Purpose":{"value":"Dummy compound"},"Batch Type":{"value":"Discovery"},"Chemist":{"value":"TestUser MCChemist"},"Description":{"value":""},"Formula Mass":{"value":"327.77 g/mol"},"Library ID":{"value":""},"Name":{"value":"ORM-0516057-001"},"Project":{"value":"Unspecified"},"Source":{"value":"Internal"},"Submission Date":{"value":"2024-10-28T17:27:56.113Z"},"Submitter":{"value":"{userId=114, userName=timo.kangasperko@orion.fi, flags={isSystemStandardUser=true}, alias=timoka, email=timo.kangasperko@orion.fi, firstName=Timo, lastName=Kangasperko, picture={}, isEnabled=true}"},"Supplier Name":{"value":"ChemDiv"},"Synthesis Date":{"value":"2011-10-10T14:48Z"}}}},{"type":"material","id":"assetType:5d6e0287ee35880008c18db5","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/assetType:5d6e0287ee35880008c18db5"},"attributes":{"type":"assetType","eid":"assetType:5d6e0287ee35880008c18db5","name":"Compounds","digest":"59951413","fields":{}}},{"type":"materialDrawing","id":"asset:671fc99b1a12207a92bcb05a","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/materials/asset:671fc99b1a12207a92bcb05a/drawing?format=cdxml"},"attributes":{"id":"asset:671fc99b1a12207a92bcb05a","type":"CHEMICAL_DRAWING"}},{"type":"user","id":"114","links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114"},"attributes":{"userId":"114","userName":"timo.kangasperko@orion.fi","flags":{"isSystemStandardUser":true},"alias":"timoka","email":"timo.kangasperko@orion.fi","firstName":"Timo","lastName":"Kangasperko","isEnabled":true},"relationships":{"systemGroups":{"links":{"self":"https://orionsandbox.signalsresearch.revvitycloud.eu/api/rest/v1.0/users/114/systemGroups"}}}}]}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>